<commit_message>
correction du tableau de comp
</commit_message>
<xml_diff>
--- a/documents/Tableau de synthèse - BTS SIO 2024.xlsx
+++ b/documents/Tableau de synthèse - BTS SIO 2024.xlsx
@@ -166,23 +166,7 @@
     <t xml:space="preserve">-Traiter des demandes concernant les applications</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
-    </r>
+    <t xml:space="preserve">-Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
   </si>
   <si>
     <t xml:space="preserve">PROJET ANDROID</t>
@@ -224,7 +208,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -309,11 +293,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -846,8 +825,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
ajout stage et projet
</commit_message>
<xml_diff>
--- a/documents/Tableau de synthèse - BTS SIO 2024.xlsx
+++ b/documents/Tableau de synthèse - BTS SIO 2024.xlsx
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
   <si>
-    <t xml:space="preserve">SESSION 2024</t>
+    <t xml:space="preserve">SESSION 2025</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
@@ -118,21 +118,7 @@
     <t xml:space="preserve">Réalisation en cours de formation</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJET PYTHON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/01/2024 
-au 
-12/01/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   - Vérifier le respect des règles d’utilisation des ressources numériques</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Planifier les activités</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJET WEB</t>
+    <t xml:space="preserve">PROJET HTML/CSS : SITE BIBLIOTHEQUE ASSOCIATIVE</t>
   </si>
   <si>
     <t xml:space="preserve">14/01/2024 au 12/04/2024</t>
@@ -144,20 +130,19 @@
     <t xml:space="preserve"> - Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJET JAVA</t>
+    <t xml:space="preserve">PROJET JAVA : APPLICATION GESTION SALARIEES </t>
   </si>
   <si>
     <t xml:space="preserve">15/01/2024 au 19/01/2024</t>
   </si>
   <si>
-    <t xml:space="preserve"> - vérifier les conditions de la continuité d’un service informatique</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Développer son projet
-professionnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJET WEB 2</t>
+    <t xml:space="preserve">-Gérer des sauvegardes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Planifier les activité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJET PHP : SITE  RECHERCHE RESTAURANT</t>
   </si>
   <si>
     <t xml:space="preserve">23/09/2024 au 10/09/2024</t>
@@ -166,19 +151,16 @@
     <t xml:space="preserve">-Traiter des demandes concernant les applications</t>
   </si>
   <si>
-    <t xml:space="preserve">-Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJET ANDROID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP PRESENTATION DES PROCESS DE L'ENTREPRISE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13/05/2024 au 21/06/2024</t>
+    <t xml:space="preserve">- Référencer les services en ligne de l’organisation et mesurer leur visibilité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Accompagner les utilisateurs dans la mise en place d’un service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJET JAVA 2 : APPLICATION GESTION SALARIEES </t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/03/2025 au 31/03/2025</t>
   </si>
   <si>
     <r>
@@ -188,7 +170,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> - </t>
+      <t xml:space="preserve">- </t>
     </r>
     <r>
       <rPr>
@@ -196,20 +178,78 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Analyser les objectifs et les modalités d’organisation d’un projet</t>
+      <t xml:space="preserve">Collecter, suivre et orienter des demandes </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> - Mettre en œuvre des outils et stratégies de veille informationnelle</t>
+    <t xml:space="preserve">-Réaliser les tests d’intégration et d’acceptation d’un service </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORTEFOLIO HTML/CSS </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Mettre en œuvre des outils et stratégies de veille informationnelle                   -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Gérer son identité professionnelle</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TP SYMFONY : LA POSTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Exploiter des référentiels, normes et standards adoptés par le prestataire informatique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
     <t xml:space="preserve">APPLICATION ACCES ANNUAIRE LDAP</t>
   </si>
   <si>
+    <t xml:space="preserve">13/05/2024 au 21/06/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mettre en place son environnement d’apprentissage personnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLICATION WEB GESTION DE TICKETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/01/2025au 14/02/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Recenser et identifier les ressources numériques </t>
+  </si>
+  <si>
     <t xml:space="preserve"> - Déployer un service</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
+    <t xml:space="preserve">SITE VITRINE SOUS WORDPRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Référencer les services en ligne de l’organisation et mesurer leur visibilité.</t>
   </si>
 </sst>
 </file>
@@ -221,7 +261,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -311,6 +351,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -630,96 +676,92 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -727,39 +769,47 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -841,10 +891,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -852,464 +902,523 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="70.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="9" style="2" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="9" style="0" width="11.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="44" style="1" width="10.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" s="17" customFormat="true" ht="324.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="15" t="s">
+    <row r="7" s="16" customFormat="true" ht="324.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" s="17" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+    <row r="8" s="16" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-    </row>
-    <row r="9" s="17" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" s="16" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-    </row>
-    <row r="11" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B12" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22" t="s">
+      <c r="E12" s="23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
+      <c r="F12" s="20"/>
+      <c r="G12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-    </row>
-    <row r="13" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
-    </row>
-    <row r="16" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
-    </row>
-    <row r="17" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" s="17" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="25" t="s">
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-    </row>
-    <row r="20" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="20" t="s">
+    </row>
+    <row r="15" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="23" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="18" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" s="16" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-    </row>
-    <row r="24" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" s="17" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
+      <c r="B20" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-    </row>
-    <row r="28" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
-    </row>
-    <row r="32" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" s="17" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="26"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="29"/>
-    </row>
-    <row r="35" s="17" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="16"/>
+      <c r="AJ20" s="16"/>
+      <c r="AK20" s="16"/>
+      <c r="AL20" s="16"/>
+      <c r="AM20" s="16"/>
+      <c r="AN20" s="16"/>
+      <c r="AO20" s="16"/>
+      <c r="AP20" s="16"/>
+      <c r="AQ20" s="16"/>
+    </row>
+    <row r="21" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" s="16" customFormat="true" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21"/>
+    </row>
+    <row r="30" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+    </row>
+    <row r="32" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+    </row>
+    <row r="33" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" s="16" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" s="16" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>